<commit_message>
mis à jour projet.xlsx
</commit_message>
<xml_diff>
--- a/Projet.xlsx
+++ b/Projet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="124">
   <si>
     <t>Access Token</t>
   </si>
@@ -367,9 +367,6 @@
     <t>Web</t>
   </si>
   <si>
-    <t>Web Wikipédia</t>
-  </si>
-  <si>
     <t>Récupérer les résultats des élections législatives 2007 et 2012</t>
   </si>
   <si>
@@ -377,6 +374,24 @@
   </si>
   <si>
     <t>Obtenir la liste des partis et leurs infos</t>
+  </si>
+  <si>
+    <t>Infos : Sexe, DatedeNaissance, Nuance, Profession, FonctionPublique, Sortant + Infos sur le suppléant</t>
+  </si>
+  <si>
+    <t>Infos : Sexe, (Inscrits, Votants, Blancs) par circo, NbrVoix</t>
+  </si>
+  <si>
+    <t>Infos :  Sexe, (Inscrits, Votants, Blancs) par circo, Nuance, NbrVoix</t>
+  </si>
+  <si>
+    <t>INSEE</t>
+  </si>
+  <si>
+    <t>Obtenir des données extérieures qui ont une influence sur les élections</t>
+  </si>
+  <si>
+    <t>Infos : Taux du chômage trimestrielle par département (2016-1982)</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1088,18 +1103,20 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" s="1"/>
@@ -1156,6 +1173,9 @@
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="D13" s="1"/>
@@ -1171,7 +1191,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1188,7 +1211,7 @@
         <v>114</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -1197,11 +1220,21 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="D19" s="1"/>

</xml_diff>

<commit_message>
add info BDD candidat
ajout des infos sur la BDD des candidats
</commit_message>
<xml_diff>
--- a/Projet.xlsx
+++ b/Projet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="24" windowWidth="19620" windowHeight="2424"/>
+    <workbookView xWindow="570" yWindow="30" windowWidth="19620" windowHeight="2430" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Steps" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="149">
   <si>
     <t>Access Token</t>
   </si>
@@ -392,13 +392,88 @@
   </si>
   <si>
     <t>Infos : Taux du chômage trimestrielle par département (2016-1982)</t>
+  </si>
+  <si>
+    <t>Libellé circonscription</t>
+  </si>
+  <si>
+    <t>N° panneau</t>
+  </si>
+  <si>
+    <t>N° candidat</t>
+  </si>
+  <si>
+    <t>Sexe candidat</t>
+  </si>
+  <si>
+    <t>Nom candidat</t>
+  </si>
+  <si>
+    <t>Prénom candidat</t>
+  </si>
+  <si>
+    <t>Date naissance candidat</t>
+  </si>
+  <si>
+    <t>Nuance candidat</t>
+  </si>
+  <si>
+    <t>Profession candidat</t>
+  </si>
+  <si>
+    <t>personnalité candidat</t>
+  </si>
+  <si>
+    <t>Le candidat est sortant</t>
+  </si>
+  <si>
+    <t>Sexe Supp.</t>
+  </si>
+  <si>
+    <t>Nom Supp.</t>
+  </si>
+  <si>
+    <t>Prénom Supp</t>
+  </si>
+  <si>
+    <t>Date naiss. Supp.</t>
+  </si>
+  <si>
+    <t>Nuance Supp.</t>
+  </si>
+  <si>
+    <t>Personnalité Supp.</t>
+  </si>
+  <si>
+    <t>Le suppléant est sortant</t>
+  </si>
+  <si>
+    <t>Copie de Leg_2017_candidatures_T1</t>
+  </si>
+  <si>
+    <t>varchar2(50)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Code du département</t>
+  </si>
+  <si>
+    <t>Libellé du département</t>
+  </si>
+  <si>
+    <t>Code circonscription</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +534,22 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -550,7 +641,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -586,11 +677,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -640,6 +768,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,16 +1211,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73.77734375" customWidth="1"/>
-    <col min="5" max="5" width="50.77734375" customWidth="1"/>
+    <col min="1" max="2" width="18.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5">
@@ -1436,10 +1584,10 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="55.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -1503,12 +1651,12 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21">
@@ -2003,15 +2151,221 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B3:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" ht="15.75">
+      <c r="B3" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="38"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="38"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2021,7 +2375,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>